<commit_message>
MS: fixing issue with Excel date/time and increased precision of all.equal for POSIXct; switching package output to display author rather than maintainer; fixed issue with querying environment variable FULL.TEST.SUITE; fixed issue with overwriting cells of different type
git-svn-id: svn://ms72.weblink.ch/mirai/XLConnect-R@257 ccc6e944-403e-a54a-b5f3-c2babcd103ea
</commit_message>
<xml_diff>
--- a/inst/unitTests/resources/testWorkbookMissingValue.xlsx
+++ b/inst/unitTests/resources/testWorkbookMissingValue.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="21315" windowHeight="9780"/>
@@ -385,7 +385,7 @@
   <dimension ref="C7:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
MS: support for numeric missing values; fixing some code and documentation issues
git-svn-id: svn://ms72.weblink.ch/mirai/XLConnect-R@281 ccc6e944-403e-a54a-b5f3-c2babcd103ea
</commit_message>
<xml_diff>
--- a/inst/unitTests/resources/testWorkbookMissingValue.xlsx
+++ b/inst/unitTests/resources/testWorkbookMissingValue.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="21315" windowHeight="9780"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="21315" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Missing1" sheetId="1" r:id="rId1"/>
+    <sheet name="Missing2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Missing1">Missing1!$C$7:$F$13</definedName>
+    <definedName name="Missing2">Missing2!$C$5:$F$11</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>A</t>
   </si>
@@ -85,9 +87,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -384,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C7:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -495,4 +498,121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C5:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="3:6">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>29921</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="C7">
+        <v>-3.2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>-9999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>29922</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="C8">
+        <v>-9999</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="2">
+        <v>-9999</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6">
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1">
+        <v>29926</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>